<commit_message>
Changed most of discussion section.
Minor edits here and there.
</commit_message>
<xml_diff>
--- a/Data/summary_data_ladybug.xlsx
+++ b/Data/summary_data_ladybug.xlsx
@@ -2,19 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Surface Evolver\Data\Bubble_Bridge\20201020 ladybug data final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adwait\Desktop\MPIP\Documents\paper-underwater_adhesion\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20970" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20970" windowHeight="9090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="adhesion" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$AF$247</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="42">
   <si>
     <t>Force_hair_air</t>
   </si>
@@ -133,11 +137,29 @@
   <si>
     <t>E:\Work\Surface Evolver\Data\Bubble_Bridge\20201020 ladybug data final\D_d=25 (ab=1.5)</t>
   </si>
+  <si>
+    <t>Adhesion</t>
+  </si>
+  <si>
+    <t>Interfacial tension old</t>
+  </si>
+  <si>
+    <t>interfacial tension new</t>
+  </si>
+  <si>
+    <t>New adhesion</t>
+  </si>
+  <si>
+    <t>Wet/Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +475,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -23709,4 +23733,529 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-0.18351022207197126</v>
+      </c>
+      <c r="B2">
+        <v>-0.11660162781978971</v>
+      </c>
+      <c r="C2">
+        <v>-0.92254829145588191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-0.49231958420420724</v>
+      </c>
+      <c r="B3">
+        <v>-0.42536457162167757</v>
+      </c>
+      <c r="C3">
+        <v>-1.4313305078559311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-0.67259746581289848</v>
+      </c>
+      <c r="B4">
+        <v>-0.60559331269693917</v>
+      </c>
+      <c r="C4">
+        <v>-1.6198822631210408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-0.6860405674951997</v>
+      </c>
+      <c r="B5">
+        <v>-0.6189705643819815</v>
+      </c>
+      <c r="C5">
+        <v>-1.5319084584213298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-0.63794576598504071</v>
+      </c>
+      <c r="B6">
+        <v>-0.57083378638234084</v>
+      </c>
+      <c r="C6">
+        <v>-1.3675815088856063</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-0.58039345613185267</v>
+      </c>
+      <c r="B7">
+        <v>-0.51324068278280033</v>
+      </c>
+      <c r="C7">
+        <v>-1.2088137825596583</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.52783122936957105</v>
+      </c>
+      <c r="B8">
+        <v>-0.46063979444976882</v>
+      </c>
+      <c r="C8">
+        <v>-1.0758008926812215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-0.4830021500754178</v>
+      </c>
+      <c r="B9">
+        <v>-0.41575859336084869</v>
+      </c>
+      <c r="C9">
+        <v>-0.96591146794810978</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-0.44617887710952697</v>
+      </c>
+      <c r="B10">
+        <v>-0.37889649630073979</v>
+      </c>
+      <c r="C10">
+        <v>-0.88545386784843927</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-0.41270886243245025</v>
+      </c>
+      <c r="B11">
+        <v>-0.34538447835608066</v>
+      </c>
+      <c r="C11">
+        <v>-0.78929150670781179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-0.38495300245023778</v>
+      </c>
+      <c r="B12">
+        <v>-0.31757777753682598</v>
+      </c>
+      <c r="C12">
+        <v>-0.73455004594080664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-0.36095732692549937</v>
+      </c>
+      <c r="B13">
+        <v>-0.29353792740494056</v>
+      </c>
+      <c r="C13">
+        <v>-0.69143913409774871</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-0.33996676007412885</v>
+      </c>
+      <c r="B14">
+        <v>-0.27250278613344359</v>
+      </c>
+      <c r="C14">
+        <v>-0.6294236526596102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-0.32145493917399359</v>
+      </c>
+      <c r="B15">
+        <v>-0.25394610050000171</v>
+      </c>
+      <c r="C15">
+        <v>-0.58716535417247007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-0.30597137177881828</v>
+      </c>
+      <c r="B16">
+        <v>-0.23841965682258606</v>
+      </c>
+      <c r="C16">
+        <v>-0.54919744447090546</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-0.29029541791322144</v>
+      </c>
+      <c r="B17">
+        <v>-0.222705874850959</v>
+      </c>
+      <c r="C17">
+        <v>-0.51514655049444891</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-0.27717926351627908</v>
+      </c>
+      <c r="B18">
+        <v>-0.20955273519618342</v>
+      </c>
+      <c r="C18">
+        <v>-0.48474118013430645</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-0.26518758982090518</v>
+      </c>
+      <c r="B19">
+        <v>-0.19752077195178705</v>
+      </c>
+      <c r="C19">
+        <v>-0.45746439382199272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-0.2542330315770604</v>
+      </c>
+      <c r="B20">
+        <v>-0.18653054399209165</v>
+      </c>
+      <c r="C20">
+        <v>-0.43266444818357291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-0.24383146023970492</v>
+      </c>
+      <c r="B21">
+        <v>-0.17608983077010956</v>
+      </c>
+      <c r="C21">
+        <v>-0.4097677888523768</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-0.23506304300520292</v>
+      </c>
+      <c r="B22">
+        <v>-0.16728364061435705</v>
+      </c>
+      <c r="C22">
+        <v>-0.38887175589508088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-0.22657219640265719</v>
+      </c>
+      <c r="B23">
+        <v>-0.15875591291703017</v>
+      </c>
+      <c r="C23">
+        <v>-0.37091067243721942</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-0.21921734168810192</v>
+      </c>
+      <c r="B24">
+        <v>-0.15136434446105762</v>
+      </c>
+      <c r="C24">
+        <v>-0.35338609035306934</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-0.21155981355982464</v>
+      </c>
+      <c r="B25">
+        <v>-0.14367070424015069</v>
+      </c>
+      <c r="C25">
+        <v>-0.33727907040059851</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-0.20512396982864983</v>
+      </c>
+      <c r="B26">
+        <v>-0.13719959016356148</v>
+      </c>
+      <c r="C26">
+        <v>-0.32192163620692371</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-0.19864123582428517</v>
+      </c>
+      <c r="B27">
+        <v>-0.13068136744465186</v>
+      </c>
+      <c r="C27">
+        <v>-0.30628192750015093</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>-0.19261380726993999</v>
+      </c>
+      <c r="B28">
+        <v>-0.12461904220017998</v>
+      </c>
+      <c r="C28">
+        <v>-0.29287143973988355</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-0.18713426886655876</v>
+      </c>
+      <c r="B29">
+        <v>-0.11910394439240693</v>
+      </c>
+      <c r="C29">
+        <v>-0.28542114139895625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>-0.18187930634311938</v>
+      </c>
+      <c r="B30">
+        <v>-0.11381243929164953</v>
+      </c>
+      <c r="C30">
+        <v>-0.26759288562061589</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>-0.17703066111798421</v>
+      </c>
+      <c r="B31">
+        <v>-0.1089315037106077</v>
+      </c>
+      <c r="C31">
+        <v>-0.25549623385501274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>-0.17236876038718646</v>
+      </c>
+      <c r="B32">
+        <v>-0.10423575141160782</v>
+      </c>
+      <c r="C32">
+        <v>-0.24604055667509769</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-0.16788080046034087</v>
+      </c>
+      <c r="B33">
+        <v>-9.9714468436928536E-2</v>
+      </c>
+      <c r="C33">
+        <v>-0.25329863748879672</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-0.16354532472936431</v>
+      </c>
+      <c r="B34">
+        <v>-9.5346398381934913E-2</v>
+      </c>
+      <c r="C34">
+        <v>-0.2257354812300601</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-0.15949225757837102</v>
+      </c>
+      <c r="B35">
+        <v>-9.1260586287944145E-2</v>
+      </c>
+      <c r="C35">
+        <v>-0.21669223311704455</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>-0.15560466636971998</v>
+      </c>
+      <c r="B36">
+        <v>-8.7341254655370765E-2</v>
+      </c>
+      <c r="C36">
+        <v>-0.20834478946340981</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>-0.15184678021198253</v>
+      </c>
+      <c r="B37">
+        <v>-8.355176008123491E-2</v>
+      </c>
+      <c r="C37">
+        <v>-0.20020780922180911</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>-6.8326159835052538E-2</v>
+      </c>
+      <c r="C38">
+        <v>-0.19237143257555517</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>-6.8356686301740244E-2</v>
+      </c>
+      <c r="C39">
+        <v>-0.18494668250213006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>-6.838666880248917E-2</v>
+      </c>
+      <c r="C40">
+        <v>-0.17884488350006206</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>-6.8416072485177948E-2</v>
+      </c>
+      <c r="C41">
+        <v>-9.6958687905157621E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>-6.8444773695119768E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ref="B45:C45" si="0">MIN(B2:B42)</f>
+        <v>-0.6189705643819815</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>-1.6198822631210408</v>
+      </c>
+      <c r="D45">
+        <f>C45/B45</f>
+        <v>2.6170586395145161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46">
+        <v>24</v>
+      </c>
+      <c r="C46">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47">
+        <v>30</v>
+      </c>
+      <c r="C47">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48">
+        <f>B45*B47/B46</f>
+        <v>-0.7737132054774768</v>
+      </c>
+      <c r="C48">
+        <f>C45*C47/C46</f>
+        <v>-1.3499018859342007</v>
+      </c>
+      <c r="D48">
+        <f>C48/B48</f>
+        <v>1.7447057596763444</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>